<commit_message>
alteração local de ponta, e add prateleira
</commit_message>
<xml_diff>
--- a/analise_curva_abc/local/datasets/local_apanha_cx.xlsx
+++ b/analise_curva_abc/local/datasets/local_apanha_cx.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estoque\Documents\estoque.renan\projetos\projeto_curva_abc\tratamento_curva_abc\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estoque\Documents\estoque.renan\projetos\projeto_curva_abc\analise_curva_abc\local\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF140FD-60EF-4F94-B1ED-BCE417BA9D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC98359-6788-4A48-8F26-40673599CD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{18EFAD8D-C71D-455A-9E0F-2475F39BFCF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$B$484</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="496">
   <si>
     <t>local</t>
   </si>
@@ -1510,6 +1513,9 @@
   </si>
   <si>
     <t>pallet</t>
+  </si>
+  <si>
+    <t>prateleira</t>
   </si>
 </sst>
 </file>
@@ -1893,7 +1899,7 @@
   <dimension ref="A1:B484"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A484" sqref="A484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4292,7 +4298,7 @@
         <v>4</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
@@ -4300,7 +4306,7 @@
         <v>11</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
@@ -4308,7 +4314,7 @@
         <v>18</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -4316,7 +4322,7 @@
         <v>25</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
@@ -4324,7 +4330,7 @@
         <v>32</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
@@ -4332,7 +4338,7 @@
         <v>39</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -4340,7 +4346,7 @@
         <v>46</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -4348,7 +4354,7 @@
         <v>53</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
@@ -4356,7 +4362,7 @@
         <v>60</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
@@ -4364,7 +4370,7 @@
         <v>67</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
@@ -4372,7 +4378,7 @@
         <v>74</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
@@ -4380,7 +4386,7 @@
         <v>81</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -4388,7 +4394,7 @@
         <v>89</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
@@ -4396,7 +4402,7 @@
         <v>97</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
@@ -4404,7 +4410,7 @@
         <v>97</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -4412,7 +4418,7 @@
         <v>111</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
@@ -4420,7 +4426,7 @@
         <v>118</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
@@ -4428,7 +4434,7 @@
         <v>125</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -4436,7 +4442,7 @@
         <v>132</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
@@ -4444,7 +4450,7 @@
         <v>139</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
@@ -4452,7 +4458,7 @@
         <v>146</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
@@ -4460,7 +4466,7 @@
         <v>153</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
@@ -4468,7 +4474,7 @@
         <v>160</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
@@ -4476,7 +4482,7 @@
         <v>167</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -4484,7 +4490,7 @@
         <v>174</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
@@ -4492,7 +4498,7 @@
         <v>179</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
@@ -4500,7 +4506,7 @@
         <v>184</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -4508,7 +4514,7 @@
         <v>189</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
@@ -4516,7 +4522,7 @@
         <v>194</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
@@ -4524,7 +4530,7 @@
         <v>199</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
@@ -4532,7 +4538,7 @@
         <v>204</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
@@ -4540,7 +4546,7 @@
         <v>209</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
@@ -4548,7 +4554,7 @@
         <v>214</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -4556,7 +4562,7 @@
         <v>219</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
@@ -4564,7 +4570,7 @@
         <v>224</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
@@ -4572,7 +4578,7 @@
         <v>229</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -4900,7 +4906,7 @@
         <v>86</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
@@ -4908,7 +4914,7 @@
         <v>94</v>
       </c>
       <c r="B375" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
@@ -4916,7 +4922,7 @@
         <v>102</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
@@ -4924,7 +4930,7 @@
         <v>108</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
@@ -4932,7 +4938,7 @@
         <v>115</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
@@ -4940,7 +4946,7 @@
         <v>122</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
@@ -4948,7 +4954,7 @@
         <v>129</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
@@ -4956,7 +4962,7 @@
         <v>136</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
@@ -4964,7 +4970,7 @@
         <v>143</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
@@ -4972,7 +4978,7 @@
         <v>150</v>
       </c>
       <c r="B383" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
@@ -5784,6 +5790,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B484" xr:uid="{E3722E28-546D-45F9-BF38-B4D5FA1D8738}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>